<commit_message>
Timer0 conflicts with millis, Timer1 for millis
</commit_message>
<xml_diff>
--- a/sch/part_list.xlsx
+++ b/sch/part_list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01.AppSource\01.Robot\B-ROBOT\sch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TJ\GitHub\02.Robot\B-ROBOT\sch\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -284,20 +284,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;₩&quot;#,##0_);[Red]\(&quot;₩&quot;#,##0\)"/>
+    <numFmt numFmtId="176" formatCode="&quot;₩&quot;#,##0_);[Red]\(&quot;₩&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -306,7 +306,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -315,7 +315,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -330,7 +330,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -454,7 +454,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -466,13 +466,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -481,10 +481,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1">
@@ -499,16 +499,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
@@ -517,16 +517,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1">
@@ -535,22 +535,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1">
@@ -570,8 +570,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -647,7 +647,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -915,16 +915,16 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="19.375" customWidth="1"/>
+    <col min="2" max="2" width="45.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.25" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.75" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.75" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" thickBot="1">
+    <row r="1" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -947,7 +947,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -969,7 +969,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -991,7 +991,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1073,7 +1073,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -1091,7 +1091,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>16</v>
       </c>
@@ -1155,7 +1155,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5" t="s">
         <v>48</v>
@@ -1172,7 +1172,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5" t="s">
         <v>58</v>
@@ -1189,7 +1189,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="22.5">
+    <row r="14" spans="1:20" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="5" t="s">
         <v>59</v>
@@ -1206,7 +1206,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="10" t="s">
         <v>60</v>
@@ -1223,7 +1223,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1239,7 +1239,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1251,7 +1251,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1263,7 +1263,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
         <v>0</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
         <v>40</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
         <v>12</v>
       </c>
@@ -1342,7 +1342,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>37</v>
       </c>
@@ -1365,7 +1365,7 @@
       </c>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
         <v>42</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
         <v>63</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="28" t="s">
         <v>61</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="28" t="s">
         <v>4</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="28" t="s">
         <v>15</v>
       </c>
@@ -1471,7 +1471,7 @@
       <c r="F27" s="28"/>
       <c r="G27" s="30"/>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="28" t="s">
         <v>17</v>
       </c>
@@ -1489,7 +1489,7 @@
       <c r="F28" s="28"/>
       <c r="G28" s="30"/>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="32" t="s">
         <v>16</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="28"/>
       <c r="B30" s="28"/>
       <c r="C30" s="28"/>
@@ -1516,7 +1516,7 @@
       <c r="F30" s="30"/>
       <c r="G30" s="30"/>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="28"/>
       <c r="B31" s="28"/>
       <c r="C31" s="28"/>
@@ -1525,7 +1525,7 @@
       <c r="F31" s="30"/>
       <c r="G31" s="30"/>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1534,22 +1534,22 @@
         <v>70440</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G43" s="35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G44" s="35" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G45" s="36" t="s">
         <v>9</v>
       </c>
@@ -1583,25 +1583,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L16"/>
+  <dimension ref="B1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.875" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>16000000</v>
       </c>
     </row>
-    <row r="3" spans="2:12">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>72</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="2:12">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E4" t="s">
         <v>67</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="2:12">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>76</v>
       </c>
@@ -1673,7 +1673,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="2:12">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>74</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="2:12">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>71</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="12" spans="2:12">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>72</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="2:12">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
         <v>67</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="14" spans="2:12">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>76</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="15" spans="2:12">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>74</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>10.869565217391305</v>
       </c>
     </row>
-    <row r="16" spans="2:12">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>71</v>
       </c>
@@ -1868,7 +1868,17 @@
         <v>4.3478260869565214E-5</v>
       </c>
     </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>1E-3</v>
+      </c>
+      <c r="C18">
+        <f>B18/C16</f>
+        <v>250.00000000000003</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
ARMs for MG90S added
</commit_message>
<xml_diff>
--- a/sch/part_list.xlsx
+++ b/sch/part_list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01.AppSource\01.Robot\B-ROBOT\sch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TJ\GitHub\02.Robot\B-ROBOT\sch\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="91">
   <si>
     <t>부품</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -246,9 +247,6 @@
     <t>LM2596 강하형 DC-DC 가변</t>
   </si>
   <si>
-    <t>AN-153 (d:88.57, h:2.62) 3개/set</t>
-  </si>
-  <si>
     <t>speed</t>
   </si>
   <si>
@@ -310,6 +308,22 @@
   </si>
   <si>
     <t>OCR</t>
+  </si>
+  <si>
+    <t>AN-152 (d:82.22, h:2.62) 3개/set</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MG-90S</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>arduino uno R3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.devicemart.co.kr/1245596</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -317,20 +331,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;₩&quot;#,##0_);[Red]\(&quot;₩&quot;#,##0\)"/>
+    <numFmt numFmtId="176" formatCode="&quot;₩&quot;#,##0_);[Red]\(&quot;₩&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -339,7 +353,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -348,7 +362,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -363,7 +377,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -394,7 +408,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -471,6 +485,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -480,14 +507,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -499,13 +526,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -514,10 +541,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1">
@@ -532,16 +559,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
@@ -550,16 +577,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1">
@@ -568,22 +595,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1">
@@ -601,10 +628,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -680,7 +719,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -942,22 +981,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T45"/>
+  <dimension ref="A1:T55"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.875" customWidth="1"/>
+    <col min="3" max="3" width="5.75" customWidth="1"/>
+    <col min="4" max="4" width="9.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.75" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15.75" thickBot="1">
+    <row r="1" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -980,7 +1020,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -1002,7 +1042,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -1024,7 +1064,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -1046,7 +1086,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
@@ -1068,7 +1108,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1090,7 +1130,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1106,7 +1146,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -1124,7 +1164,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
@@ -1146,7 +1186,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
@@ -1168,7 +1208,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>16</v>
       </c>
@@ -1188,7 +1228,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="5" t="s">
         <v>48</v>
@@ -1205,7 +1245,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="5" t="s">
         <v>58</v>
@@ -1222,7 +1262,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="22.5">
+    <row r="14" spans="1:20" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="5" t="s">
         <v>59</v>
@@ -1239,7 +1279,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="10" t="s">
         <v>60</v>
@@ -1256,7 +1296,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1272,7 +1312,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1284,7 +1324,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1296,7 +1336,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
         <v>0</v>
       </c>
@@ -1325,7 +1365,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
         <v>40</v>
       </c>
@@ -1353,7 +1393,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
         <v>12</v>
       </c>
@@ -1375,7 +1415,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>37</v>
       </c>
@@ -1398,7 +1438,7 @@
       </c>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
         <v>42</v>
       </c>
@@ -1420,7 +1460,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
         <v>63</v>
       </c>
@@ -1442,12 +1482,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="28" t="s">
         <v>61</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="C25" s="28">
         <v>1</v>
@@ -1464,7 +1504,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="28" t="s">
         <v>4</v>
       </c>
@@ -1486,7 +1526,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" s="28" t="s">
         <v>15</v>
       </c>
@@ -1504,7 +1544,7 @@
       <c r="F27" s="28"/>
       <c r="G27" s="30"/>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="28" t="s">
         <v>17</v>
       </c>
@@ -1522,137 +1562,609 @@
       <c r="F28" s="28"/>
       <c r="G28" s="30"/>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="32"/>
+      <c r="B29" s="32" t="s">
+        <v>88</v>
+      </c>
       <c r="C29" s="32">
-        <v>2</v>
-      </c>
-      <c r="D29" s="33"/>
+        <v>1</v>
+      </c>
+      <c r="D29" s="33">
+        <v>2690</v>
+      </c>
       <c r="E29" s="34">
         <f>C27*D29</f>
+        <v>2690</v>
+      </c>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="E30" s="2">
+        <f>SUM(E20:E29)</f>
+        <v>73130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A32" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20">
-      <c r="A30" s="28"/>
-      <c r="B30" s="28"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="30"/>
-    </row>
-    <row r="31" spans="1:20">
-      <c r="A31" s="28"/>
-      <c r="B31" s="28"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-    </row>
-    <row r="32" spans="1:20">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="E32" s="2">
-        <f>SUM(E20:E31)</f>
-        <v>70440</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="G43" s="35" t="s">
+      <c r="B32" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" s="40" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="S32" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="T32" s="37">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A33" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C33" s="24">
+        <v>1</v>
+      </c>
+      <c r="D33" s="25">
+        <v>6300</v>
+      </c>
+      <c r="E33" s="26">
+        <f>C33*D33</f>
+        <v>6300</v>
+      </c>
+      <c r="F33" s="41"/>
+      <c r="G33" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="S33" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="T33" s="37">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A34" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="24">
+        <v>1</v>
+      </c>
+      <c r="D34" s="25">
+        <v>2700</v>
+      </c>
+      <c r="E34" s="26">
+        <f t="shared" ref="E34:E39" si="4">C34*D34</f>
+        <v>2700</v>
+      </c>
+      <c r="F34" s="41"/>
+      <c r="G34" s="27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A35" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="24">
+        <v>1</v>
+      </c>
+      <c r="D35" s="25">
+        <v>24000</v>
+      </c>
+      <c r="E35" s="26">
+        <f t="shared" si="4"/>
+        <v>24000</v>
+      </c>
+      <c r="F35" s="41"/>
+      <c r="G35" s="27" t="s">
+        <v>46</v>
+      </c>
+      <c r="L35" s="1"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A36" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="24">
+        <v>1</v>
+      </c>
+      <c r="D36" s="25">
+        <v>2700</v>
+      </c>
+      <c r="E36" s="26">
+        <f t="shared" si="4"/>
+        <v>2700</v>
+      </c>
+      <c r="F36" s="41"/>
+      <c r="G36" s="27" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A37" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="28">
+        <v>1</v>
+      </c>
+      <c r="D37" s="29">
+        <v>3000</v>
+      </c>
+      <c r="E37" s="31">
+        <f>C37*D37</f>
+        <v>3000</v>
+      </c>
+      <c r="F37" s="42"/>
+      <c r="G37" s="35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A38" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="28">
+        <v>1</v>
+      </c>
+      <c r="D38" s="29">
+        <v>1000</v>
+      </c>
+      <c r="E38" s="29">
+        <f>C38*D38</f>
+        <v>1000</v>
+      </c>
+      <c r="F38" s="42"/>
+      <c r="G38" s="35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A39" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="28">
+        <v>2</v>
+      </c>
+      <c r="D39" s="29">
+        <v>13020</v>
+      </c>
+      <c r="E39" s="29">
+        <f t="shared" ref="E39:E43" si="5">C39*D39</f>
+        <v>26040</v>
+      </c>
+      <c r="F39" s="43"/>
+      <c r="G39" s="35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A40" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" s="28">
+        <v>1</v>
+      </c>
+      <c r="D40" s="29"/>
+      <c r="E40" s="31">
+        <f t="shared" ref="E40" si="6">C39*D40</f>
+        <v>0</v>
+      </c>
+      <c r="F40" s="43"/>
+      <c r="G40" s="30"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A41" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="28">
+        <v>1</v>
+      </c>
+      <c r="D41" s="29"/>
+      <c r="E41" s="31">
+        <f>C42*D41</f>
+        <v>0</v>
+      </c>
+      <c r="F41" s="43"/>
+      <c r="G41" s="30"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A42" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="32">
+        <v>1</v>
+      </c>
+      <c r="D42" s="33">
+        <v>2690</v>
+      </c>
+      <c r="E42" s="34">
+        <f>C40*D42</f>
+        <v>2690</v>
+      </c>
+      <c r="F42" s="42"/>
+      <c r="G42" s="30"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A43" s="28"/>
+      <c r="B43" s="28"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29">
+        <f>SUM(E33:E42)</f>
+        <v>68430</v>
+      </c>
+    </row>
+    <row r="53" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G53" s="35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
-      <c r="G44" s="35" t="s">
+    <row r="54" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G54" s="35" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
-      <c r="G45" s="36" t="s">
+    <row r="55" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G55" s="36" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G45" r:id="rId1"/>
-    <hyperlink ref="G44" r:id="rId2"/>
-    <hyperlink ref="G3" r:id="rId3"/>
-    <hyperlink ref="G5" r:id="rId4"/>
-    <hyperlink ref="G7" r:id="rId5"/>
-    <hyperlink ref="G43" r:id="rId6"/>
-    <hyperlink ref="G6" r:id="rId7"/>
-    <hyperlink ref="G10" r:id="rId8"/>
-    <hyperlink ref="G9" r:id="rId9"/>
-    <hyperlink ref="G2" r:id="rId10"/>
-    <hyperlink ref="G22" r:id="rId11"/>
-    <hyperlink ref="G21" r:id="rId12"/>
-    <hyperlink ref="G23" r:id="rId13"/>
-    <hyperlink ref="G26" r:id="rId14"/>
-    <hyperlink ref="G20" r:id="rId15"/>
-    <hyperlink ref="G25" r:id="rId16"/>
-    <hyperlink ref="G24" r:id="rId17"/>
+    <hyperlink ref="G3" r:id="rId1"/>
+    <hyperlink ref="G5" r:id="rId2"/>
+    <hyperlink ref="G7" r:id="rId3"/>
+    <hyperlink ref="G6" r:id="rId4"/>
+    <hyperlink ref="G10" r:id="rId5"/>
+    <hyperlink ref="G9" r:id="rId6"/>
+    <hyperlink ref="G2" r:id="rId7"/>
+    <hyperlink ref="G22" r:id="rId8"/>
+    <hyperlink ref="G21" r:id="rId9"/>
+    <hyperlink ref="G23" r:id="rId10"/>
+    <hyperlink ref="G26" r:id="rId11"/>
+    <hyperlink ref="G20" r:id="rId12"/>
+    <hyperlink ref="G25" r:id="rId13"/>
+    <hyperlink ref="G24" r:id="rId14"/>
+    <hyperlink ref="G53" r:id="rId15"/>
+    <hyperlink ref="G54" r:id="rId16"/>
+    <hyperlink ref="G55" r:id="rId17"/>
+    <hyperlink ref="G35" r:id="rId18"/>
+    <hyperlink ref="G34" r:id="rId19"/>
+    <hyperlink ref="G36" r:id="rId20"/>
+    <hyperlink ref="G39" r:id="rId21"/>
+    <hyperlink ref="G38" r:id="rId22"/>
+    <hyperlink ref="G37" r:id="rId23"/>
+    <hyperlink ref="G33" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
-  <drawing r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId25"/>
+  <drawing r:id="rId26"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="24">
+        <v>1</v>
+      </c>
+      <c r="D2" s="26">
+        <v>6300</v>
+      </c>
+      <c r="E2" s="26">
+        <f>C2*D2</f>
+        <v>6300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="24">
+        <v>1</v>
+      </c>
+      <c r="D3" s="26">
+        <v>2700</v>
+      </c>
+      <c r="E3" s="26">
+        <f t="shared" ref="E3:E8" si="0">C3*D3</f>
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="24">
+        <v>1</v>
+      </c>
+      <c r="D4" s="26">
+        <v>24000</v>
+      </c>
+      <c r="E4" s="26">
+        <f t="shared" si="0"/>
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="24">
+        <v>1</v>
+      </c>
+      <c r="D5" s="26">
+        <v>2700</v>
+      </c>
+      <c r="E5" s="26">
+        <f t="shared" si="0"/>
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="28">
+        <v>1</v>
+      </c>
+      <c r="D6" s="31">
+        <v>3000</v>
+      </c>
+      <c r="E6" s="31">
+        <f>C6*D6</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="28">
+        <v>1</v>
+      </c>
+      <c r="D7" s="31">
+        <v>1000</v>
+      </c>
+      <c r="E7" s="31">
+        <f>C7*D7</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="28">
+        <v>2</v>
+      </c>
+      <c r="D8" s="31">
+        <v>13020</v>
+      </c>
+      <c r="E8" s="31">
+        <f t="shared" ref="E8:E12" si="1">C8*D8</f>
+        <v>26040</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="28">
+        <v>1</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31">
+        <f t="shared" ref="E9" si="2">C8*D9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="28">
+        <v>1</v>
+      </c>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31">
+        <f>C11*D10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="32">
+        <v>1</v>
+      </c>
+      <c r="D11" s="34">
+        <v>2690</v>
+      </c>
+      <c r="E11" s="34">
+        <f>C9*D11</f>
+        <v>2690</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31">
+        <f>SUM(E2:E11)</f>
+        <v>68430</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.875" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12">
+    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>16000000</v>
       </c>
     </row>
-    <row r="3" spans="2:12">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3">
         <v>8</v>
       </c>
       <c r="F3" t="s">
+        <v>67</v>
+      </c>
+      <c r="L3" t="s">
         <v>68</v>
       </c>
-      <c r="L3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12">
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F4">
         <v>-500</v>
@@ -1673,15 +2185,15 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="2:12">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F5">
         <f>F4*C5</f>
@@ -1708,16 +2220,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="2:12">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="38">
         <f>B1/C3</f>
         <v>2000000</v>
       </c>
       <c r="E6" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F6">
         <f>C6/F5</f>
@@ -1740,16 +2252,16 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="2:12">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7">
         <f>1/C6</f>
         <v>4.9999999999999998E-7</v>
       </c>
       <c r="E7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H7">
         <f>C7*H6</f>
@@ -1768,23 +2280,23 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="12" spans="2:12">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12">
         <v>1024</v>
       </c>
       <c r="F12" t="s">
+        <v>67</v>
+      </c>
+      <c r="L12" t="s">
         <v>68</v>
       </c>
-      <c r="L12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12">
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="E13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F13">
         <v>-500</v>
@@ -1802,21 +2314,21 @@
         <v>250</v>
       </c>
       <c r="K13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L13">
         <v>500</v>
       </c>
     </row>
-    <row r="14" spans="2:12">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C14">
         <v>46</v>
       </c>
       <c r="E14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F14">
         <f>F13*C14</f>
@@ -1843,16 +2355,16 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="15" spans="2:12">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C15" s="38">
         <f>B1/C12</f>
         <v>15625</v>
       </c>
       <c r="E15" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F15">
         <f>C15/F14</f>
@@ -1875,16 +2387,16 @@
         <v>0.67934782608695654</v>
       </c>
     </row>
-    <row r="16" spans="2:12">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C16">
         <f>1/C15</f>
         <v>6.3999999999999997E-5</v>
       </c>
       <c r="E16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H16">
         <f>C16*H15</f>
@@ -1903,7 +2415,7 @@
         <v>4.3478260869565214E-5</v>
       </c>
     </row>
-    <row r="18" spans="2:9">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>1.6299999999999999E-2</v>
       </c>
@@ -1912,7 +2424,7 @@
         <v>254.6875</v>
       </c>
     </row>
-    <row r="19" spans="2:9">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C19">
         <f>C16*256</f>
         <v>1.6383999999999999E-2</v>
@@ -1922,9 +2434,9 @@
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:9">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1945,9 +2457,9 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="22" spans="2:9">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1956,7 +2468,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="23" spans="2:9">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E23">
         <f>E21/(I21-D21)*(I22-D22)</f>
         <v>7.8125</v>
@@ -1974,7 +2486,7 @@
         <v>31.25</v>
       </c>
     </row>
-    <row r="24" spans="2:9">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E24">
         <f>E23*C16</f>
         <v>5.0000000000000001E-4</v>
@@ -1992,36 +2504,36 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="26" spans="2:9">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E26" t="s">
+        <v>83</v>
+      </c>
+      <c r="F26" t="s">
         <v>84</v>
       </c>
-      <c r="F26" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9">
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" t="s">
         <v>77</v>
-      </c>
-      <c r="C27" t="s">
-        <v>78</v>
       </c>
       <c r="D27">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="2:9">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D28">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="2:9">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D29">
         <v>12.6</v>
@@ -2035,7 +2547,7 @@
         <v>0.315</v>
       </c>
     </row>
-    <row r="30" spans="2:9">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D30">
         <v>13.2</v>
       </c>
@@ -2048,19 +2560,19 @@
         <v>0.32999999999999996</v>
       </c>
     </row>
-    <row r="34" spans="2:2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="2:2">
-      <c r="B35" t="s">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2">
-      <c r="B36" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
esp8266 at command processor added
</commit_message>
<xml_diff>
--- a/sch/part_list.xlsx
+++ b/sch/part_list.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TJ\GitHub\02.Robot\B-ROBOT\sch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\01.AppSource\01.Robot\B-ROBOT\sch\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13185" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13185" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -331,20 +331,20 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="&quot;₩&quot;#,##0_);[Red]\(&quot;₩&quot;#,##0\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;₩&quot;#,##0_);[Red]\(&quot;₩&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -353,7 +353,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -362,7 +362,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -377,7 +377,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -514,7 +514,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -526,13 +526,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -541,10 +541,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1">
@@ -559,16 +559,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
@@ -577,16 +577,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1">
@@ -595,22 +595,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1">
@@ -642,8 +642,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="하이퍼링크" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -719,7 +719,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -983,21 +983,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T55"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A32" sqref="A32:E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.875" customWidth="1"/>
-    <col min="3" max="3" width="5.75" customWidth="1"/>
-    <col min="4" max="4" width="9.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.75" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" ht="15.75" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20">
       <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1146,7 +1146,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -1164,7 +1164,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20">
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
@@ -1186,7 +1186,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20">
       <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20">
       <c r="A11" s="18" t="s">
         <v>16</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20">
       <c r="A12" s="5"/>
       <c r="B12" s="5" t="s">
         <v>48</v>
@@ -1245,7 +1245,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20">
       <c r="A13" s="5"/>
       <c r="B13" s="5" t="s">
         <v>58</v>
@@ -1262,7 +1262,7 @@
         <v>5.8</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="22.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" ht="22.5">
       <c r="A14" s="5"/>
       <c r="B14" s="5" t="s">
         <v>59</v>
@@ -1279,7 +1279,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20">
       <c r="A15" s="10"/>
       <c r="B15" s="10" t="s">
         <v>60</v>
@@ -1296,7 +1296,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1312,7 +1312,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1324,7 +1324,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1336,7 +1336,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20">
       <c r="A19" s="22" t="s">
         <v>0</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20">
       <c r="A20" s="24" t="s">
         <v>40</v>
       </c>
@@ -1393,7 +1393,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20">
       <c r="A21" s="24" t="s">
         <v>12</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20">
       <c r="A22" s="24" t="s">
         <v>37</v>
       </c>
@@ -1438,7 +1438,7 @@
       </c>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20">
       <c r="A23" s="24" t="s">
         <v>42</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20">
       <c r="A24" s="28" t="s">
         <v>63</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20">
       <c r="A25" s="28" t="s">
         <v>61</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20">
       <c r="A26" s="28" t="s">
         <v>4</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20">
       <c r="A27" s="28" t="s">
         <v>15</v>
       </c>
@@ -1544,7 +1544,7 @@
       <c r="F27" s="28"/>
       <c r="G27" s="30"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20">
       <c r="A28" s="28" t="s">
         <v>17</v>
       </c>
@@ -1562,7 +1562,7 @@
       <c r="F28" s="28"/>
       <c r="G28" s="30"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20">
       <c r="A29" s="32" t="s">
         <v>16</v>
       </c>
@@ -1582,7 +1582,7 @@
       <c r="F29" s="30"/>
       <c r="G29" s="30"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1591,12 +1591,12 @@
         <v>73130</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20">
       <c r="A32" s="22" t="s">
         <v>0</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20">
       <c r="A33" s="24" t="s">
         <v>40</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20">
       <c r="A34" s="24" t="s">
         <v>12</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>2700</v>
       </c>
       <c r="E34" s="26">
-        <f t="shared" ref="E34:E39" si="4">C34*D34</f>
+        <f t="shared" ref="E34:E36" si="4">C34*D34</f>
         <v>2700</v>
       </c>
       <c r="F34" s="41"/>
@@ -1675,7 +1675,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20">
       <c r="A35" s="24" t="s">
         <v>37</v>
       </c>
@@ -1698,7 +1698,7 @@
       </c>
       <c r="L35" s="1"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20">
       <c r="A36" s="24" t="s">
         <v>42</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20">
       <c r="A37" s="28" t="s">
         <v>63</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20">
       <c r="A38" s="28" t="s">
         <v>61</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20">
       <c r="A39" s="28" t="s">
         <v>4</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>13020</v>
       </c>
       <c r="E39" s="29">
-        <f t="shared" ref="E39:E43" si="5">C39*D39</f>
+        <f t="shared" ref="E39" si="5">C39*D39</f>
         <v>26040</v>
       </c>
       <c r="F39" s="43"/>
@@ -1786,7 +1786,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20">
       <c r="A40" s="28" t="s">
         <v>15</v>
       </c>
@@ -1804,7 +1804,7 @@
       <c r="F40" s="43"/>
       <c r="G40" s="30"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20">
       <c r="A41" s="28" t="s">
         <v>17</v>
       </c>
@@ -1822,7 +1822,7 @@
       <c r="F41" s="43"/>
       <c r="G41" s="30"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20">
       <c r="A42" s="32" t="s">
         <v>16</v>
       </c>
@@ -1842,7 +1842,7 @@
       <c r="F42" s="42"/>
       <c r="G42" s="30"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20">
       <c r="A43" s="28"/>
       <c r="B43" s="28"/>
       <c r="C43" s="28"/>
@@ -1852,17 +1852,17 @@
         <v>68430</v>
       </c>
     </row>
-    <row r="53" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="7:7">
       <c r="G53" s="35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="7:7">
       <c r="G54" s="35" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="7:7">
       <c r="G55" s="36" t="s">
         <v>9</v>
       </c>
@@ -1905,19 +1905,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" s="24" t="s">
         <v>40</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>6300</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" s="24" t="s">
         <v>12</v>
       </c>
@@ -1966,11 +1966,11 @@
         <v>2700</v>
       </c>
       <c r="E3" s="26">
-        <f t="shared" ref="E3:E8" si="0">C3*D3</f>
+        <f t="shared" ref="E3:E5" si="0">C3*D3</f>
         <v>2700</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" s="24" t="s">
         <v>37</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" s="24" t="s">
         <v>42</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" s="28" t="s">
         <v>63</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" s="28" t="s">
         <v>61</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" s="28" t="s">
         <v>4</v>
       </c>
@@ -2056,11 +2056,11 @@
         <v>13020</v>
       </c>
       <c r="E8" s="31">
-        <f t="shared" ref="E8:E12" si="1">C8*D8</f>
+        <f t="shared" ref="E8" si="1">C8*D8</f>
         <v>26040</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" s="28" t="s">
         <v>15</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" s="28" t="s">
         <v>17</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" s="32" t="s">
         <v>16</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>2690</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" s="28"/>
       <c r="B12" s="28"/>
       <c r="C12" s="28"/>
@@ -2130,25 +2130,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.875" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12">
       <c r="B1">
         <v>16000000</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12">
       <c r="B3" t="s">
         <v>71</v>
       </c>
@@ -2162,7 +2162,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12">
       <c r="E4" t="s">
         <v>66</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12">
       <c r="B5" t="s">
         <v>75</v>
       </c>
@@ -2220,7 +2220,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12">
       <c r="B6" t="s">
         <v>73</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12">
       <c r="B7" t="s">
         <v>70</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12">
       <c r="B12" t="s">
         <v>71</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12">
       <c r="E13" t="s">
         <v>66</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12">
       <c r="B14" t="s">
         <v>75</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>23000</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12">
       <c r="B15" t="s">
         <v>73</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>0.67934782608695654</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12">
       <c r="B16" t="s">
         <v>70</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>4.3478260869565214E-5</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9">
       <c r="B18">
         <v>1.6299999999999999E-2</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>254.6875</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9">
       <c r="C19">
         <f>C16*256</f>
         <v>1.6383999999999999E-2</v>
@@ -2434,7 +2434,7 @@
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9">
       <c r="C21" t="s">
         <v>85</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9">
       <c r="C22" t="s">
         <v>86</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9">
       <c r="E23">
         <f>E21/(I21-D21)*(I22-D22)</f>
         <v>7.8125</v>
@@ -2486,7 +2486,7 @@
         <v>31.25</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9">
       <c r="E24">
         <f>E23*C16</f>
         <v>5.0000000000000001E-4</v>
@@ -2504,7 +2504,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9">
       <c r="E26" t="s">
         <v>83</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9">
       <c r="B27" t="s">
         <v>76</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9">
       <c r="C28" t="s">
         <v>78</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9">
       <c r="C29" t="s">
         <v>79</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>0.315</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9">
       <c r="D30">
         <v>13.2</v>
       </c>
@@ -2560,17 +2560,26 @@
         <v>0.32999999999999996</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9">
+      <c r="D31">
+        <v>20</v>
+      </c>
+      <c r="E31">
+        <f>D28/(D27+D28)*D31</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
       <c r="B34" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2">
       <c r="B35" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2">
       <c r="B36" t="s">
         <v>82</v>
       </c>

</xml_diff>

<commit_message>
batt voltage divider resistors added
R1, R2 added
</commit_message>
<xml_diff>
--- a/sch/part_list.xlsx
+++ b/sch/part_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13185" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13185" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2130,8 +2130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2520,7 +2520,7 @@
         <v>77</v>
       </c>
       <c r="D27">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="2:9">
@@ -2528,7 +2528,7 @@
         <v>78</v>
       </c>
       <c r="D28">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="2:9">
@@ -2540,11 +2540,11 @@
       </c>
       <c r="E29">
         <f>D28/(D27+D28)*D29</f>
-        <v>3.15</v>
+        <v>4.1999999999999993</v>
       </c>
       <c r="F29">
         <f>D29/(D27+D28)</f>
-        <v>0.315</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="30" spans="2:9">
@@ -2553,16 +2553,16 @@
       </c>
       <c r="E30">
         <f>D28/(D27+D28)*D30</f>
-        <v>3.3</v>
+        <v>4.3999999999999995</v>
       </c>
       <c r="F30">
         <f>D30/(D27+D28)</f>
-        <v>0.32999999999999996</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="31" spans="2:9">
       <c r="D31">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E31">
         <f>D28/(D27+D28)*D31</f>

</xml_diff>